<commit_message>
Modified screen shot function
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Webview_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Webview_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="85">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -561,36 +561,6 @@
 validate7;</t>
   </si>
   <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate4
-{
-validate_Text_Exists=VT200-0985
-};
-validate5
-{
-validate_Screenshot=VT200_beforenavigateback
-};
-validate6
-{
-validate_Text_Exists=VT200-0986
-};
-validate7
-{
-validate_Screenshot=VT200_0986
-};</t>
-  </si>
-  <si>
     <t xml:space="preserve">validate1
 {
 validate_PageTitle=Compliance JS specs
@@ -795,6 +765,152 @@
 };</t>
   </si>
   <si>
+    <t>Get enableCache as True</t>
+  </si>
+  <si>
+    <t>get webviewFramework</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0991_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+validate4;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0991
+};
+validate4
+{
+validate_SystemProperties=webviewFramework
+};</t>
+  </si>
+  <si>
+    <t>Do not set enableCache in Rhoconfig txt</t>
+  </si>
+  <si>
+    <t>Get enableCache as false</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0988_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+validate4;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0988
+};
+validate4
+{
+validate_Result=true
+};</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0989_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+validate4;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0989
+};
+validate4
+{
+validate_Result=true
+};</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0990_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+validate4;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0990
+};
+validate4
+{
+validate_Result=true
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0990
+};
+validate4
+{
+validate_Result=false
+};</t>
+  </si>
+  <si>
     <t>wait(3);
 validate1;
 link_Click(webview_test_link);
@@ -812,159 +928,12 @@
 wait(2);
 SwitchApp(WEBVIEW);
 wait(2);
-SelectTestToRun(VT200_0981_string);
+SelectTestToRun(VT200_0979_string);
 ClickRunTest(runtest_top_xpath);
 validate4;
 ClickRunTest(runtest_bottom_xpath);
 wait(3);
-CheckUITextContains(Tab_2);
-CheckUITextContains(Hello);</t>
-  </si>
-  <si>
-    <t>Get enableCache as True</t>
-  </si>
-  <si>
-    <t>get webviewFramework</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0991_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-validate4;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0991
-};
-validate4
-{
-validate_SystemProperties=webviewFramework
-};</t>
-  </si>
-  <si>
-    <t>Do not set enableCache in Rhoconfig txt</t>
-  </si>
-  <si>
-    <t>Get enableCache as false</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0988_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-validate4;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0988
-};
-validate4
-{
-validate_Result=true
-};</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0989_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-validate4;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0989
-};
-validate4
-{
-validate_Result=true
-};</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0990_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-validate4;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0990
-};
-validate4
-{
-validate_Result=true
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0990
-};
-validate4
-{
-validate_Result=false
-};</t>
+validate5;</t>
   </si>
   <si>
     <t>wait(3);
@@ -978,18 +947,67 @@
 wait(3);
 SwitchApp(NATIVE_APP);
 wait(2);
-link_Click(VT200_0976_tab1_xpath);
+link_Click(VT200_0976_tab4_xpath);
 wait(2);
 link_Click(VT200_0976_tab0_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
 wait(2);
-SelectTestToRun(VT200_0979_string);
+SelectTestToRun(VT200_0978_string);
 ClickRunTest(runtest_top_xpath);
 validate4;
 ClickRunTest(runtest_bottom_xpath);
 wait(3);
 validate5;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate5
+{
+validate_Text_Exists=VT200-0978
+};
+validate6
+{
+validate_Result=http://127.0.0.1
+validate_Result=app/WebviewNew/Page4.html
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate5
+{
+validate_Screenshot=VT200_0987_before
+};
+validate6
+{
+validate_Text_Exists=VT200-0987
+};
+validate7
+{
+validate_Screenshot=VT200_0987_after
+};</t>
   </si>
   <si>
     <t>wait(3);
@@ -1000,21 +1018,24 @@
 ClickRunTest(runtest_top_xpath);
 validate3;
 ClickRunTest(runtest_bottom_xpath);
-wait(3);
 SwitchApp(NATIVE_APP);
 wait(2);
-link_Click(VT200_0976_tab4_xpath);
-wait(2);
+link_Click(VT200_0976_tab1_xpath);
+wait(10);
+TakeNativeScreenshot(VT200_0987_before);
+validate5;
 link_Click(VT200_0976_tab0_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
 wait(2);
-SelectTestToRun(VT200_0978_string);
-ClickRunTest(runtest_top_xpath);
-validate4;
-ClickRunTest(runtest_bottom_xpath);
-wait(3);
-validate5;</t>
+SelectTestToRun(VT200_0987_string);
+ClickRunTest(runtest_top_xpath);
+validate6;
+ClickRunTest(runtest_bottom_xpath);
+SwitchApp(NATIVE_APP);
+link_Click(VT200_0976_tab1_xpath);
+TakeNativeScreenshot(VT200_0987_after);
+validate7;</t>
   </si>
   <si>
     <t>validate1
@@ -1029,40 +1050,21 @@
 {
 validate_Text_Exists=VT200-0976
 };
+validate4
+{
+validate_Text_Exists=VT200-0985
+};
 validate5
 {
-validate_Text_Exists=VT200-0978
+validate_Screenshot=VT200_0985beforenavigateback
 };
 validate6
 {
-validate_Result=http://127.0.0.1
-validate_Result=app/WebviewNew/Page4.html
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate5
-{
-validate_Screenshot=VT200_0987_before
-};
-validate6
-{
-validate_Text_Exists=VT200-0987
+validate_Text_Exists=VT200-0986
 };
 validate7
 {
-validate_Screenshot=VT200_0987_after
+validate_Screenshot=VT200_0986
 };</t>
   </si>
   <si>
@@ -1074,37 +1076,27 @@
 ClickRunTest(runtest_top_xpath);
 validate3;
 ClickRunTest(runtest_bottom_xpath);
+wait(3);
 SwitchApp(NATIVE_APP);
 wait(2);
 link_Click(VT200_0976_tab1_xpath);
-wait(10);
-TakeNativeScreenshot(VT200_0987_before);
-validate5;
+wait(2);
 link_Click(VT200_0976_tab0_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
 wait(2);
-SelectTestToRun(VT200_0987_string);
-ClickRunTest(runtest_top_xpath);
-validate6;
-ClickRunTest(runtest_bottom_xpath);
-SwitchApp(NATIVE_APP);
-link_Click(VT200_0976_tab1_xpath);
-TakeNativeScreenshot(VT200_0987_after);
-validate7;</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Pass</t>
+SelectTestToRun(VT200_0981_string);
+ClickRunTest(runtest_top_xpath);
+validate4;
+ClickRunTest(runtest_bottom_xpath);
+wait(3);
+CheckUITextContains(Hello);</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -1500,19 +1492,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="40.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.02265625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="35" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="35.25" thickBot="1">
@@ -1579,9 +1569,7 @@
       <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:12" ht="203.25" thickBot="1">
@@ -1608,9 +1596,7 @@
         <v>38</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="248.25" thickBot="1">
@@ -1629,15 +1615,13 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="293.25" thickBot="1">
@@ -1658,15 +1642,13 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="225.75" thickBot="1">
@@ -1693,9 +1675,7 @@
         <v>32</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="225.75" thickBot="1">
@@ -1722,9 +1702,7 @@
         <v>30</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="225.75" thickBot="1">
@@ -1735,9 +1713,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1751,9 +1727,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:12" ht="180.75" thickBot="1">
@@ -1764,9 +1738,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1774,15 +1746,13 @@
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="225.75" thickBot="1">
@@ -1793,9 +1763,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1830,15 +1798,13 @@
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="214.5" thickBot="1">
@@ -1859,15 +1825,13 @@
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="214.5" thickBot="1">
@@ -1886,15 +1850,13 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="259.5" thickBot="1">
@@ -1915,15 +1877,13 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="259.5" thickBot="1">
@@ -1944,15 +1904,13 @@
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="203.25" thickBot="1">
@@ -1973,18 +1931,16 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="270.75" thickBot="1">
+    <row r="17" spans="1:11" ht="259.5" thickBot="1">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2002,15 +1958,13 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="315.75" thickBot="1">
@@ -2031,15 +1985,13 @@
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="409.6" thickBot="1">
@@ -2063,12 +2015,10 @@
         <v>53</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="I19" s="2"/>
-      <c r="J19" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="270.75" thickBot="1">
@@ -2095,9 +2045,7 @@
         <v>51</v>
       </c>
       <c r="I20" s="2"/>
-      <c r="J20" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="270.75" thickBot="1">
@@ -2124,9 +2072,7 @@
         <v>49</v>
       </c>
       <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="180.75" thickBot="1">
@@ -2141,19 +2087,17 @@
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I22" s="2"/>
-      <c r="J22" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="180.75" thickBot="1">
@@ -2168,19 +2112,17 @@
         <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I23" s="2"/>
-      <c r="J23" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" ht="180.75" thickBot="1">
@@ -2195,19 +2137,17 @@
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I24" s="2"/>
-      <c r="J24" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" ht="180.75" thickBot="1">
@@ -2222,19 +2162,17 @@
         <v>10</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I25" s="2"/>
-      <c r="J25" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" ht="180.75" thickBot="1">
@@ -2249,14 +2187,14 @@
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>

</xml_diff>

<commit_message>
Modified DSl in webview
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Webview_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Webview_JS.xlsx
@@ -516,6 +516,356 @@
 validate5;</t>
   </si>
   <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate4
+{
+validate_Text_Exists=VT200-0985
+};
+validate5
+{
+validate_Screenshot=VT200_0985
+};
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0976_string);
+ClickRunTest(runtest_top_xpath);
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+SwitchApp(NATIVE_APP);
+wait(2);
+link_Click(VT200_0976_tab1_xpath);
+wait(2);
+link_Click(VT200_0976_tab0_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+wait(2);
+SelectTestToRun(VT200_0985_string);
+ClickRunTest(runtest_top_xpath);
+validate4;
+ClickRunTest(runtest_bottom_xpath);
+wait(3);
+SwitchApp(NATIVE_APP);
+wait(2);
+link_Click(VT200_0976_tab1_xpath);
+wait(4);
+TakeNativeScreenshot(VT200_0985);
+validate5;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0980_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(3);
+validate5;
+</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate4
+{
+validate_Text_Exists=VT200-0979
+};
+validate5
+{
+validate_Result=http://127.0.0.1:
+validate_Result=app/WebviewTest/Page1.html
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_1004_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+validate4;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_1003_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+validate4;
+</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_1000_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+validate4;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-1000
+};
+validate4
+{
+validate_Result=true
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_1002_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+validate4;
+TakeScreenshot(VT200_1002_before);
+ZoomPage(body_xpath);
+wait(2);
+TakeScreenshot(VT200-1002);
+validate5;
+</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-1002
+};
+validate4
+{
+validate_Result=1. enable_screen_zoom set value is 0
+validate_Result=2. WebView enableZoom value is false
+};
+validate5
+{
+validate_Screenshot=VT200_1002_before
+validate_Screenshot=VT200-1002
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate4
+{
+validate_Text_Exists=VT200-0981
+};</t>
+  </si>
+  <si>
+    <t>Get enableCache as True</t>
+  </si>
+  <si>
+    <t>get webviewFramework</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0991_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+validate4;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0991
+};
+validate4
+{
+validate_SystemProperties=webviewFramework
+};</t>
+  </si>
+  <si>
+    <t>Do not set enableCache in Rhoconfig txt</t>
+  </si>
+  <si>
+    <t>Get enableCache as false</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0988_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+validate4;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0988
+};
+validate4
+{
+validate_Result=true
+};</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0989_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+validate4;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0989
+};
+validate4
+{
+validate_Result=true
+};</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0990_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+validate4;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0990
+};
+validate4
+{
+validate_Result=true
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0990
+};
+validate4
+{
+validate_Result=false
+};</t>
+  </si>
+  <si>
     <t>wait(3);
 validate1;
 link_Click(webview_test_link);
@@ -524,391 +874,21 @@
 ClickRunTest(runtest_top_xpath);
 validate3;
 ClickRunTest(runtest_bottom_xpath);
-wait(2);
-SwitchApp(NATIVE_APP);
-wait(2);
-link_Click(VT200_0976_tab1_xpath);
-wait(2);
-link_Click(VT200_0976_tab0_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-wait(2);
-SelectTestToRun(VT200_0985_string);
-ClickRunTest(runtest_top_xpath);
-validate4;
-ClickRunTest(runtest_bottom_xpath);
 wait(3);
 SwitchApp(NATIVE_APP);
 wait(2);
 link_Click(VT200_0976_tab1_xpath);
-wait(5);
-TakeNativeScreenshot(VT200_beforenavigateback);
-validate5;
+wait(2);
 link_Click(VT200_0976_tab0_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
 wait(2);
-SelectTestToRun(VT200_0986_string);
-ClickRunTest(runtest_top_xpath);
-validate6;
+SelectTestToRun(VT200_0979_string);
+ClickRunTest(runtest_top_xpath);
+validate4;
 ClickRunTest(runtest_bottom_xpath);
 wait(3);
-SwitchApp(NATIVE_APP);
-wait(2);
-link_Click(VT200_0976_tab1_xpath);
-wait(4);
-TakeNativeScreenshot(VT200_0986);
-validate7;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate4
-{
-validate_Text_Exists=VT200-0985
-};
-validate5
-{
-validate_Screenshot=VT200_0985
-};
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0976_string);
-ClickRunTest(runtest_top_xpath);
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-SwitchApp(NATIVE_APP);
-wait(2);
-link_Click(VT200_0976_tab1_xpath);
-wait(2);
-link_Click(VT200_0976_tab0_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-wait(2);
-SelectTestToRun(VT200_0985_string);
-ClickRunTest(runtest_top_xpath);
-validate4;
-ClickRunTest(runtest_bottom_xpath);
-wait(3);
-SwitchApp(NATIVE_APP);
-wait(2);
-link_Click(VT200_0976_tab1_xpath);
-wait(4);
-TakeNativeScreenshot(VT200_0985);
-validate5;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0980_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(3);
-validate5;
-</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate4
-{
-validate_Text_Exists=VT200-0979
-};
-validate5
-{
-validate_Result=http://127.0.0.1:
-validate_Result=app/WebviewTest/Page1.html
-};</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_1004_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-validate4;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_1003_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-validate4;
-</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_1000_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-validate4;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-1000
-};
-validate4
-{
-validate_Result=true
-};</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_1002_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-validate4;
-TakeScreenshot(VT200_1002_before);
-ZoomPage(body_xpath);
-wait(2);
-TakeScreenshot(VT200-1002);
-validate5;
-</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-1002
-};
-validate4
-{
-validate_Result=1. enable_screen_zoom set value is 0
-validate_Result=2. WebView enableZoom value is false
-};
-validate5
-{
-validate_Screenshot=VT200_1002_before
-validate_Screenshot=VT200-1002
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate4
-{
-validate_Text_Exists=VT200-0981
-};</t>
-  </si>
-  <si>
-    <t>Get enableCache as True</t>
-  </si>
-  <si>
-    <t>get webviewFramework</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0991_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-validate4;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0991
-};
-validate4
-{
-validate_SystemProperties=webviewFramework
-};</t>
-  </si>
-  <si>
-    <t>Do not set enableCache in Rhoconfig txt</t>
-  </si>
-  <si>
-    <t>Get enableCache as false</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0988_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-validate4;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0988
-};
-validate4
-{
-validate_Result=true
-};</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0989_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-validate4;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0989
-};
-validate4
-{
-validate_Result=true
-};</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0990_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-validate4;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0990
-};
-validate4
-{
-validate_Result=true
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0990
-};
-validate4
-{
-validate_Result=false
-};</t>
+validate5;</t>
   </si>
   <si>
     <t>wait(3);
@@ -922,18 +902,67 @@
 wait(3);
 SwitchApp(NATIVE_APP);
 wait(2);
-link_Click(VT200_0976_tab1_xpath);
+link_Click(VT200_0976_tab4_xpath);
 wait(2);
 link_Click(VT200_0976_tab0_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
 wait(2);
-SelectTestToRun(VT200_0979_string);
+SelectTestToRun(VT200_0978_string);
 ClickRunTest(runtest_top_xpath);
 validate4;
 ClickRunTest(runtest_bottom_xpath);
 wait(3);
 validate5;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate5
+{
+validate_Text_Exists=VT200-0978
+};
+validate6
+{
+validate_Result=http://127.0.0.1
+validate_Result=app/WebviewNew/Page4.html
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate5
+{
+validate_Screenshot=VT200_0987_before
+};
+validate6
+{
+validate_Text_Exists=VT200-0987
+};
+validate7
+{
+validate_Screenshot=VT200_0987_after
+};</t>
   </si>
   <si>
     <t>wait(3);
@@ -944,70 +973,24 @@
 ClickRunTest(runtest_top_xpath);
 validate3;
 ClickRunTest(runtest_bottom_xpath);
-wait(3);
 SwitchApp(NATIVE_APP);
 wait(2);
-link_Click(VT200_0976_tab4_xpath);
-wait(2);
+link_Click(VT200_0976_tab1_xpath);
+wait(10);
+TakeNativeScreenshot(VT200_0987_before);
+validate5;
 link_Click(VT200_0976_tab0_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
 wait(2);
-SelectTestToRun(VT200_0978_string);
-ClickRunTest(runtest_top_xpath);
-validate4;
-ClickRunTest(runtest_bottom_xpath);
-wait(3);
-validate5;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate5
-{
-validate_Text_Exists=VT200-0978
-};
-validate6
-{
-validate_Result=http://127.0.0.1
-validate_Result=app/WebviewNew/Page4.html
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate5
-{
-validate_Screenshot=VT200_0987_before
-};
-validate6
-{
-validate_Text_Exists=VT200-0987
-};
-validate7
-{
-validate_Screenshot=VT200_0987_after
-};</t>
+SelectTestToRun(VT200_0987_string);
+ClickRunTest(runtest_top_xpath);
+validate6;
+ClickRunTest(runtest_bottom_xpath);
+SwitchApp(NATIVE_APP);
+link_Click(VT200_0976_tab1_xpath);
+TakeNativeScreenshot(VT200_0987_after);
+validate7;</t>
   </si>
   <si>
     <t>wait(3);
@@ -1018,54 +1001,21 @@
 ClickRunTest(runtest_top_xpath);
 validate3;
 ClickRunTest(runtest_bottom_xpath);
+wait(3);
 SwitchApp(NATIVE_APP);
 wait(2);
 link_Click(VT200_0976_tab1_xpath);
-wait(10);
-TakeNativeScreenshot(VT200_0987_before);
-validate5;
+wait(2);
 link_Click(VT200_0976_tab0_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
 wait(2);
-SelectTestToRun(VT200_0987_string);
-ClickRunTest(runtest_top_xpath);
-validate6;
-ClickRunTest(runtest_bottom_xpath);
-SwitchApp(NATIVE_APP);
-link_Click(VT200_0976_tab1_xpath);
-TakeNativeScreenshot(VT200_0987_after);
-validate7;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Webview JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate4
-{
-validate_Text_Exists=VT200-0985
-};
-validate5
-{
-validate_Screenshot=VT200_0985beforenavigateback
-};
-validate6
-{
-validate_Text_Exists=VT200-0986
-};
-validate7
-{
-validate_Screenshot=VT200_0986
-};</t>
+SelectTestToRun(VT200_0981_string);
+ClickRunTest(runtest_top_xpath);
+validate4;
+ClickRunTest(runtest_bottom_xpath);
+wait(3);
+CheckUITextContains(Hello);</t>
   </si>
   <si>
     <t>wait(3);
@@ -1076,21 +1026,61 @@
 ClickRunTest(runtest_top_xpath);
 validate3;
 ClickRunTest(runtest_bottom_xpath);
+wait(2);
+SwitchApp(NATIVE_APP);
+wait(2);
+link_Click(VT200_0976_tab1_xpath);
+wait(2);
+link_Click(VT200_0976_tab0_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+wait(2);
+SelectTestToRun(VT200_0985_string);
+ClickRunTest(runtest_top_xpath);
+validate4;
+ClickRunTest(runtest_bottom_xpath);
 wait(3);
 SwitchApp(NATIVE_APP);
 wait(2);
 link_Click(VT200_0976_tab1_xpath);
-wait(2);
+wait(5);
+CheckUITextContains(Google);
 link_Click(VT200_0976_tab0_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
 wait(2);
-SelectTestToRun(VT200_0981_string);
-ClickRunTest(runtest_top_xpath);
-validate4;
+SelectTestToRun(VT200_0986_string);
+ClickRunTest(runtest_top_xpath);
+validate6;
 ClickRunTest(runtest_bottom_xpath);
 wait(3);
-CheckUITextContains(Hello);</t>
+SwitchApp(NATIVE_APP);
+wait(2);
+link_Click(VT200_0976_tab1_xpath);
+wait(4);
+CheckUITextContains(Page1);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Webview JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate4
+{
+validate_Text_Exists=VT200-0985
+};
+validate6
+{
+validate_Text_Exists=VT200-0986
+};</t>
   </si>
 </sst>
 </file>
@@ -1492,7 +1482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1615,10 +1607,10 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1642,10 +1634,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1746,10 +1738,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1798,7 +1790,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>39</v>
@@ -1825,7 +1817,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>40</v>
@@ -1850,7 +1842,7 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>42</v>
@@ -1877,10 +1869,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1904,10 +1896,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1931,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>35</v>
@@ -1958,10 +1950,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1985,10 +1977,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -2012,10 +2004,10 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -2087,14 +2079,14 @@
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -2112,14 +2104,14 @@
         <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -2137,14 +2129,14 @@
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2162,14 +2154,14 @@
         <v>10</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2187,14 +2179,14 @@
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>

</xml_diff>

<commit_message>
Added fix for VT985 test in DSL
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Webview_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Webview_JS.xlsx
@@ -990,39 +990,48 @@
 ClickRunTest(runtest_top_xpath);
 validate3;
 ClickRunTest(runtest_bottom_xpath);
-wait(2);
-SwitchApp(NATIVE_APP);
-wait(2);
-ClickNativeIcon(VT200_0976_tab1_xpath);
-wait(2);
-ClickNativeIcon(VT200_0976_tab0_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-wait(2);
-SelectTestToRun(VT200_0985_string);
-ClickRunTest(runtest_top_xpath);
-validate4;
-ClickRunTest(runtest_bottom_xpath);
 wait(3);
 SwitchApp(NATIVE_APP);
 wait(2);
 ClickNativeIcon(VT200_0976_tab1_xpath);
-wait(5);
-CheckUITextContains(Google);
+wait(2);
 ClickNativeIcon(VT200_0976_tab0_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
 wait(2);
-SelectTestToRun(VT200_0986_string);
-ClickRunTest(runtest_top_xpath);
-validate6;
+SelectTestToRun(VT200_0983_string);
+ClickRunTest(runtest_top_xpath);
+wait(3);
+validate4;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+validate5;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0976_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
 ClickRunTest(runtest_bottom_xpath);
 wait(3);
 SwitchApp(NATIVE_APP);
 wait(2);
 ClickNativeIcon(VT200_0976_tab1_xpath);
-wait(4);
-CheckUITextContains(Page1);</t>
+wait(2);
+ClickNativeIcon(VT200_0976_tab0_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+wait(2);
+SelectTestToRun(VT200_0977_string);
+ClickRunTest(runtest_top_xpath);
+validate4;
+ClickRunTest(runtest_bottom_xpath);
+wait(5);
+validate5;
+</t>
   </si>
   <si>
     <t>wait(3);
@@ -1033,48 +1042,40 @@
 ClickRunTest(runtest_top_xpath);
 validate3;
 ClickRunTest(runtest_bottom_xpath);
+wait(2);
+SwitchApp(NATIVE_APP);
+wait(2);
+ClickNativeIcon(VT200_0976_tab1_xpath);
+wait(2);
+ClickNativeIcon(VT200_0976_tab0_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+wait(2);
+SelectTestToRun(VT200_0985_string);
+ClickRunTest(runtest_top_xpath);
+validate4;
+ClickRunTest(runtest_bottom_xpath);
 wait(3);
 SwitchApp(NATIVE_APP);
 wait(2);
 ClickNativeIcon(VT200_0976_tab1_xpath);
-wait(2);
+wait(5);
+CheckUITextContains(Google);
 ClickNativeIcon(VT200_0976_tab0_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
 wait(2);
-SelectTestToRun(VT200_0983_string);
-ClickRunTest(runtest_top_xpath);
-wait(3);
-validate4;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-validate5;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0976_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
+ScrollUp_Page(body_xpath);
+SelectTestToRun(VT200_0986_string);
+ClickRunTest(runtest_top_xpath);
+validate6;
 ClickRunTest(runtest_bottom_xpath);
 wait(3);
 SwitchApp(NATIVE_APP);
 wait(2);
 ClickNativeIcon(VT200_0976_tab1_xpath);
-wait(2);
-ClickNativeIcon(VT200_0976_tab0_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-wait(2);
-SelectTestToRun(VT200_0977_string);
-ClickRunTest(runtest_top_xpath);
-validate4;
-ClickRunTest(runtest_bottom_xpath);
-wait(5);
-validate5;
-</t>
+wait(4);
+CheckUITextContains(Page1);</t>
   </si>
 </sst>
 </file>
@@ -1476,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1998,7 +1999,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>75</v>
@@ -2025,7 +2026,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>50</v>
@@ -2052,7 +2053,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>49</v>

</xml_diff>